<commit_message>
Extended the microservice for course
</commit_message>
<xml_diff>
--- a/services/users/professor.xlsx
+++ b/services/users/professor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>Courses</t>
+  </si>
+  <si>
+    <t>dragos_gavrilut@gmail.com</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Gavriluț Dragoș</t>
+  </si>
+  <si>
+    <t>Lenuta Alboaie</t>
+  </si>
+  <si>
+    <t>Lect. Dr.</t>
+  </si>
+  <si>
+    <t>lenuta_alboaie@gmail.com</t>
+  </si>
+  <si>
+    <t>Retele de calculatoare, Cloud Computing</t>
   </si>
 </sst>
 </file>
@@ -371,18 +392,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="39.5703125" customWidth="1"/>
     <col min="7" max="7" width="43.42578125" customWidth="1"/>
@@ -416,9 +437,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>